<commit_message>
put rpm excel overview in template
</commit_message>
<xml_diff>
--- a/src/soliddriver_checks/config/templates/templates.xlsx
+++ b/src/soliddriver_checks/config/templates/templates.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Solid driver check result (Drivers)</t>
   </si>
@@ -37,14 +37,35 @@
 SUSE Release: this driver was built for which SUSE OS version</t>
   </si>
   <si>
-    <t>RPM-checks</t>
+    <t>Solid driver check result (RPMs)</t>
+  </si>
+  <si>
+    <t>soliddriver-checks is a tool for parnter(s) and customer(s) to check their RPMs to ensure these are meet basic SUSE requirements.</t>
+  </si>
+  <si>
+    <t>Please refer to Kernel Module Packages Manual to learn how to build a KMP(Kernel Module Package).</t>
+  </si>
+  <si>
+    <t>What do we check?</t>
+  </si>
+  <si>
+    <t>supported flag: 'yes' means this package is built by SUSE and supported by SUSE, 'external' means this package is built by vendor and supported by both SUSE and vendor, 'Missing' or others means this package does not contain 'supported' flag or unrecognizable 'supported' flag, please contact your IHV or who provide this package to you, we don't recommend you install it.</t>
+  </si>
+  <si>
+    <t>symbol check: For all KMP packages, the symbols needed by the drivers in this packages, should also have the requires in RPM and the checksum should match. Otherwise we don't recommend you install it.</t>
+  </si>
+  <si>
+    <t>signature: We list it here but not check if it's from the vendor in the list, please veirfy it by youself.</t>
+  </si>
+  <si>
+    <t>vendor: SUSE partner who provides and supports the kernel module code and packaging.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -64,6 +85,28 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font/>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14.0"/>
+      <color theme="1"/>
+      <name val="Poppins"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="&quot;poppins medium&quot;"/>
     </font>
   </fonts>
   <fills count="4">
@@ -86,13 +129,57 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border/>
+    <border>
+      <left/>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -105,8 +192,27 @@
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1344,12 +1450,12 @@
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A2:S2"/>
+    <mergeCell ref="A3:S4"/>
+    <mergeCell ref="A5:S5"/>
+    <mergeCell ref="A6:S6"/>
+    <mergeCell ref="A7:S7"/>
     <mergeCell ref="A8:S8"/>
-    <mergeCell ref="A7:S7"/>
-    <mergeCell ref="A6:S6"/>
-    <mergeCell ref="A3:S4"/>
-    <mergeCell ref="A2:S2"/>
-    <mergeCell ref="A5:S5"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
@@ -1367,13 +1473,151 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="10" max="10" width="35.63"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="12"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A7:J7"/>
+  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
enhance html/excel output format
</commit_message>
<xml_diff>
--- a/src/soliddriver_checks/config/templates/templates.xlsx
+++ b/src/soliddriver_checks/config/templates/templates.xlsx
@@ -3,73 +3,72 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="driver-check-summary" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="rpm-check-summary" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="km-report-overview" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="kmp-report-overview" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mjoq5DtJ93llYgEHczv4zIs5ceZTg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mi+AX4EaElpJr0HpzOtuedqH2FcSQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Solid driver check result (Drivers)</t>
+    <t>soliddriver check report (Kernel Module)</t>
   </si>
   <si>
-    <t>soliddriver-checks is a tool for parnter(s) and customer(s) to check their drivers installed and RPMs to ensure these are meet basic SUSE requirements.</t>
+    <r>
+      <rPr>
+        <rFont val="Poppins"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve">soliddriver-checks is a tool for parnter and customer to check their KMPs(Kernel Module Packages) or installed/running kernel modules whether can meet basic SUSE requirements. More information can be found at: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Poppins"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://github.com/SUSE/soliddriver-checks</t>
+    </r>
   </si>
   <si>
-    <t>What do we check for drivers?</t>
+    <t>soliddriver check report (Kernel Module Packages)</t>
   </si>
   <si>
-    <t>supported flag:
-    'yes' means this package is built by SUSE and supported by SUSE
-    'external' means this package is built by vendor and supported by both SUSE and vendor
-    'Missing' or others means this package does not contain 'supported' flag or unrecognizable 'supported' flag
-    Please contact your IHV or who provide this package to you if it's highlighted, we don't recommend you install it.
-RPM information: means which RPM have this driver installed
-SUSE Release: this driver was built for which SUSE OS version</t>
-  </si>
-  <si>
-    <t>Solid driver check result (RPMs)</t>
-  </si>
-  <si>
-    <t>soliddriver-checks is a tool for parnter(s) and customer(s) to check their RPMs to ensure these are meet basic SUSE requirements.</t>
-  </si>
-  <si>
-    <t>Please refer to Kernel Module Packages Manual to learn how to build a KMP(Kernel Module Package).</t>
-  </si>
-  <si>
-    <t>What do we check?</t>
-  </si>
-  <si>
-    <t>supported flag: 'yes' means this package is built by SUSE and supported by SUSE, 'external' means this package is built by vendor and supported by both SUSE and vendor, 'Missing' or others means this package does not contain 'supported' flag or unrecognizable 'supported' flag, please contact your IHV or who provide this package to you, we don't recommend you install it.</t>
-  </si>
-  <si>
-    <t>symbol check: For all KMP packages, the symbols needed by the drivers in this packages, should also have the requires in RPM and the checksum should match. Otherwise we don't recommend you install it.</t>
-  </si>
-  <si>
-    <t>signature: We list it here but not check if it's from the vendor in the list, please veirfy it by youself.</t>
-  </si>
-  <si>
-    <t>vendor: SUSE partner who provides and supports the kernel module code and packaging.</t>
+    <r>
+      <rPr>
+        <rFont val="Poppins"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve">soliddriver-checks is a tool for parnter and customer to check their KMPs(Kernel Module Packages) or installed/running kernel modules whether can meet basic SUSE requirements. More information can be found at: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Poppins"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://github.com/SUSE/soliddriver-checks</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -78,7 +77,17 @@
       <name val="Poppins"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="14.0"/>
+      <color rgb="FF000000"/>
+      <name val="Poppins"/>
+    </font>
+    <font>
+      <u/>
       <color rgb="FF000000"/>
       <name val="Poppins"/>
     </font>
@@ -87,26 +96,8 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="18.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font/>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14.0"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Poppins"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="&quot;poppins medium&quot;"/>
     </font>
   </fonts>
   <fills count="4">
@@ -129,90 +120,28 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="1">
     <border/>
-    <border>
-      <left/>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <right/>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -273,14 +202,14 @@
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="calibri"/>
-        <a:ea typeface="calibri"/>
-        <a:cs typeface="calibri"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="calibri"/>
-        <a:ea typeface="calibri"/>
-        <a:cs typeface="calibri"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -434,39 +363,163 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="39.5"/>
-    <col customWidth="1" min="2" max="26" width="7.63"/>
+    <col customWidth="1" min="1" max="1" width="95.75"/>
+    <col customWidth="1" min="2" max="2" width="59.75"/>
+    <col customWidth="1" min="3" max="26" width="7.63"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="2"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="6"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
     </row>
     <row r="5">
-      <c r="A5" s="3"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="A6" s="7"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="2"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
     </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
+    <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1"/>
     <row r="25" ht="15.75" customHeight="1"/>
     <row r="26" ht="15.75" customHeight="1"/>
@@ -1446,21 +1499,14 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
     <row r="1002" ht="15.75" customHeight="1"/>
-    <row r="1003" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="A2:S2"/>
-    <mergeCell ref="A3:S4"/>
-    <mergeCell ref="A5:S5"/>
-    <mergeCell ref="A6:S6"/>
-    <mergeCell ref="A7:S7"/>
-    <mergeCell ref="A8:S8"/>
-  </mergeCells>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="A3"/>
+  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1474,150 +1520,214 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="106.75"/>
+    <col customWidth="1" min="2" max="2" width="68.13"/>
     <col customWidth="1" min="10" max="10" width="35.63"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
+      <c r="A1" s="1" t="s">
+        <v>2</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="6"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
-        <v>5</v>
+      <c r="A3" s="5" t="s">
+        <v>3</v>
       </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
     </row>
     <row r="5">
-      <c r="A5" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="A5" s="7"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="12"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
     </row>
     <row r="8">
-      <c r="A8" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="12"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="12"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10">
-      <c r="A10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
     </row>
     <row r="11">
-      <c r="A11" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="12"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A8:J8"/>
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="A10:J10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A7:J7"/>
-  </mergeCells>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="A3"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add kmp xlsx report support
</commit_message>
<xml_diff>
--- a/src/soliddriver_checks/config/templates/templates.xlsx
+++ b/src/soliddriver_checks/config/templates/templates.xlsx
@@ -1,14 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26008"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{702D9744-4B0A-4114-A285-45C4E4764F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="km-report-overview" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="kmp-report-overview" sheetId="2" r:id="rId5"/>
+    <sheet name="km-report-overview" sheetId="1" r:id="rId1"/>
+    <sheet name="kmp-report-overview" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mi+AX4EaElpJr0HpzOtuedqH2FcSQ=="/>
     </ext>
@@ -17,23 +32,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>soliddriver check report (Kernel Module)</t>
   </si>
   <si>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Poppins"/>
-        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve">soliddriver-checks is a tool for parnter and customer to check their KMPs(Kernel Module Packages) or installed/running kernel modules whether can meet basic SUSE requirements. More information can be found at: </t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Poppins"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>https://github.com/SUSE/soliddriver-checks</t>
     </r>
@@ -41,71 +58,54 @@
   <si>
     <t>soliddriver check report (Kernel Module Packages)</t>
   </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Poppins"/>
-        <color rgb="FF000000"/>
-      </rPr>
-      <t xml:space="preserve">soliddriver-checks is a tool for parnter and customer to check their KMPs(Kernel Module Packages) or installed/running kernel modules whether can meet basic SUSE requirements. More information can be found at: </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Poppins"/>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>https://github.com/SUSE/soliddriver-checks</t>
-    </r>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Poppins"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Poppins"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Poppins"/>
     </font>
     <font>
       <u/>
-      <color rgb="FF000000"/>
-      <name val="Poppins"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color rgb="FF1155CC"/>
       <name val="Poppins"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -113,54 +113,50 @@
         <bgColor rgb="FF30BA78"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEFEFEF"/>
-        <bgColor rgb="FFEFEFEF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -350,174 +346,176 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="95.75"/>
-    <col customWidth="1" min="2" max="2" width="59.75"/>
-    <col customWidth="1" min="3" max="26" width="7.63"/>
+    <col min="1" max="1" width="95.75" customWidth="1"/>
+    <col min="2" max="2" width="59.75" customWidth="1"/>
+    <col min="3" max="26" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:19" ht="27.75" customHeight="1">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:19" ht="21.75">
       <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
     </row>
-    <row r="3">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:19" ht="57">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
     </row>
-    <row r="4">
-      <c r="A4" s="6"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
+    <row r="4" spans="1:19" ht="21.75">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
     </row>
-    <row r="5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
+    <row r="5" spans="1:19" ht="21.75">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
     </row>
-    <row r="6">
-      <c r="A6" s="7"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
+    <row r="6" spans="1:19" ht="21.75">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
     </row>
-    <row r="7">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
+    <row r="7" spans="1:19">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
     </row>
     <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1"/>
@@ -1501,233 +1499,232 @@
     <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A3"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <printOptions/>
-  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="106.75"/>
-    <col customWidth="1" min="2" max="2" width="68.13"/>
-    <col customWidth="1" min="10" max="10" width="35.63"/>
+    <col min="1" max="1" width="106.75" customWidth="1"/>
+    <col min="2" max="2" width="68.125" customWidth="1"/>
+    <col min="10" max="10" width="35.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:19" ht="29.25" customHeight="1">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:19" ht="21.75">
       <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
     </row>
-    <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
+    <row r="3" spans="1:19" ht="57">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
     </row>
-    <row r="4">
-      <c r="A4" s="6"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
+    <row r="4" spans="1:19" ht="21.75">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
     </row>
-    <row r="5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
+    <row r="5" spans="1:19" ht="21.75">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
     </row>
-    <row r="6">
-      <c r="A6" s="7"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
+    <row r="6" spans="1:19" ht="21.75">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
     </row>
-    <row r="7">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
+    <row r="7" spans="1:19">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
     </row>
-    <row r="8">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+    <row r="8" spans="1:19">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
     </row>
-    <row r="9">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+    <row r="9" spans="1:19">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
     </row>
-    <row r="10">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+    <row r="10" spans="1:19">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
     </row>
-    <row r="11">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
+    <row r="11" spans="1:19">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A3"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
</xml_diff>